<commit_message>
FEAT: ADDED COMMON FEATURES DATA TO DATASET
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/Desktop/Proyectos/Trabajo/Técnico 2023 (corto)/Notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/Desktop/Proyectos/Trabajo/Técnico 2023 (corto)/saas-pricing/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B76CEAC-CBEB-4740-948B-9ABB4B868484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3CCCF2-FA95-C24A-A2D6-30161C3C67C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>saasName</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Overleaf</t>
+  </si>
+  <si>
+    <t>numberOfCommonFeatures</t>
   </si>
 </sst>
 </file>
@@ -160,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -283,11 +286,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,11 +332,55 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -697,13 +757,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -741,6 +794,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -789,20 +849,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:I26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I26" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{49B744FF-135F-FB49-8E67-3ADFF62F7F62}" name="informationFeatures" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{1B62A5E0-E167-3145-9233-957D202AC16A}" name="integrationFeatures" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{CEACD7F9-49A9-9E45-8D00-FFC8B5A30D0D}" name="toolFeatures" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0222289F-50F8-9242-832F-7A98C3ED517F}" name="automationFeatures" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{3195318E-BB70-0B45-A51D-5FD62E35192E}" name="managementFeatures" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5275409F-8C49-954E-A147-3656249FC072}" name="numberOfFeatures" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:J26" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:J26" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{49B744FF-135F-FB49-8E67-3ADFF62F7F62}" name="informationFeatures" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1B62A5E0-E167-3145-9233-957D202AC16A}" name="integrationFeatures" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{CEACD7F9-49A9-9E45-8D00-FFC8B5A30D0D}" name="toolFeatures" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{0222289F-50F8-9242-832F-7A98C3ED517F}" name="automationFeatures" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{3195318E-BB70-0B45-A51D-5FD62E35192E}" name="managementFeatures" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{5275409F-8C49-954E-A147-3656249FC072}" name="numberOfFeatures" dataDxfId="2">
       <calculatedColumnFormula>SUM(C2:G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{129E0E18-6600-354E-AD0E-5A7A34201D39}" name="numberOfAddOns" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{129E0E18-6600-354E-AD0E-5A7A34201D39}" name="numberOfAddOns" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{BFFF5A20-56DB-2A47-AB0B-063517490554}" name="numberOfCommonFeatures" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1105,18 +1166,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="38" customWidth="1"/>
+    <col min="1" max="10" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1144,8 +1206,11 @@
       <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1174,8 +1239,11 @@
       <c r="I2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1204,8 +1272,11 @@
       <c r="I3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1234,8 +1305,11 @@
       <c r="I4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1264,8 +1338,11 @@
       <c r="I5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1294,8 +1371,11 @@
       <c r="I6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1324,8 +1404,11 @@
       <c r="I7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1354,8 +1437,11 @@
       <c r="I8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1384,8 +1470,11 @@
       <c r="I9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1414,8 +1503,11 @@
       <c r="I10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1444,8 +1536,11 @@
       <c r="I11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1474,8 +1569,11 @@
       <c r="I12" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1504,8 +1602,11 @@
       <c r="I13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1534,8 +1635,11 @@
       <c r="I14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1564,8 +1668,11 @@
       <c r="I15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1594,8 +1701,11 @@
       <c r="I16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1624,8 +1734,11 @@
       <c r="I17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1654,8 +1767,11 @@
       <c r="I18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1684,8 +1800,11 @@
       <c r="I19" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1714,8 +1833,11 @@
       <c r="I20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1744,8 +1866,11 @@
       <c r="I21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1774,8 +1899,11 @@
       <c r="I22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
@@ -1804,8 +1932,11 @@
       <c r="I23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1834,8 +1965,11 @@
       <c r="I24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -1864,8 +1998,11 @@
       <c r="I25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -1894,9 +2031,12 @@
       <c r="I26" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="J26" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
FEAT: ADDED NUMBER OF PLANS DATA TO DATASET
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/Desktop/Proyectos/Trabajo/Técnico 2023 (corto)/saas-pricing/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3CCCF2-FA95-C24A-A2D6-30161C3C67C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853BFE1D-DF11-6449-A922-BF077AAC21C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>saasName</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>numberOfCommonFeatures</t>
+  </si>
+  <si>
+    <t>numberOfPlans</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -849,21 +893,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:J26" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:J26" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{49B744FF-135F-FB49-8E67-3ADFF62F7F62}" name="informationFeatures" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1B62A5E0-E167-3145-9233-957D202AC16A}" name="integrationFeatures" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{CEACD7F9-49A9-9E45-8D00-FFC8B5A30D0D}" name="toolFeatures" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{0222289F-50F8-9242-832F-7A98C3ED517F}" name="automationFeatures" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{3195318E-BB70-0B45-A51D-5FD62E35192E}" name="managementFeatures" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{5275409F-8C49-954E-A147-3656249FC072}" name="numberOfFeatures" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K26" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{49B744FF-135F-FB49-8E67-3ADFF62F7F62}" name="informationFeatures" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{1B62A5E0-E167-3145-9233-957D202AC16A}" name="integrationFeatures" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{CEACD7F9-49A9-9E45-8D00-FFC8B5A30D0D}" name="toolFeatures" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{0222289F-50F8-9242-832F-7A98C3ED517F}" name="automationFeatures" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{3195318E-BB70-0B45-A51D-5FD62E35192E}" name="managementFeatures" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{5275409F-8C49-954E-A147-3656249FC072}" name="numberOfFeatures" dataDxfId="3">
       <calculatedColumnFormula>SUM(C2:G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{129E0E18-6600-354E-AD0E-5A7A34201D39}" name="numberOfAddOns" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{BFFF5A20-56DB-2A47-AB0B-063517490554}" name="numberOfCommonFeatures" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{129E0E18-6600-354E-AD0E-5A7A34201D39}" name="numberOfAddOns" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{BFFF5A20-56DB-2A47-AB0B-063517490554}" name="numberOfCommonFeatures" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{7C71CB94-471E-4642-BC09-7715792BEAD6}" name="numberOfPlans" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1166,19 +1211,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M23" sqref="M23"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="38" customWidth="1"/>
+    <col min="1" max="11" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1209,8 +1254,11 @@
       <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1242,8 +1290,11 @@
       <c r="J2" s="10">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1275,8 +1326,11 @@
       <c r="J3" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1308,8 +1362,11 @@
       <c r="J4" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1341,8 +1398,11 @@
       <c r="J5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1374,8 +1434,11 @@
       <c r="J6" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1407,8 +1470,11 @@
       <c r="J7" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1440,8 +1506,11 @@
       <c r="J8" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1473,8 +1542,11 @@
       <c r="J9" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1506,8 +1578,11 @@
       <c r="J10" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1539,8 +1614,11 @@
       <c r="J11" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1572,8 +1650,11 @@
       <c r="J12" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1603,10 +1684,13 @@
         <v>0</v>
       </c>
       <c r="J13" s="1">
+        <v>19</v>
+      </c>
+      <c r="K13" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1636,10 +1720,13 @@
         <v>0</v>
       </c>
       <c r="J14" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1671,8 +1758,11 @@
       <c r="J15" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1704,8 +1794,11 @@
       <c r="J16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1737,8 +1830,11 @@
       <c r="J17" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1770,8 +1866,11 @@
       <c r="J18" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1803,8 +1902,11 @@
       <c r="J19" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1836,8 +1938,11 @@
       <c r="J20" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1869,8 +1974,11 @@
       <c r="J21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1902,8 +2010,11 @@
       <c r="J22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
@@ -1935,8 +2046,11 @@
       <c r="J23" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1968,8 +2082,11 @@
       <c r="J24" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -2001,8 +2118,11 @@
       <c r="J25" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2034,9 +2154,12 @@
       <c r="J26" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="K26" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
docs: 2019, 2020 data collected
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/Desktop/Proyectos/Trabajo/Técnico 2023 (corto)/saas-pricing/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\PlanModels\saas-pricing\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853BFE1D-DF11-6449-A922-BF077AAC21C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957A8714-F0F9-4C7B-A5E8-F89D63255502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>saasName</t>
   </si>
@@ -893,8 +893,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K26" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K41" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K41" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2020"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:K41">
+    <sortCondition ref="A1:A41"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="9"/>
@@ -1211,19 +1220,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M24" sqref="M24"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="11" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1294,7 +1303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1330,7 +1339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1402,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1546,7 +1555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1618,7 +1627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1726,403 +1735,403 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1">
         <v>2019</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
+        <v>17</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(C15:G15)</f>
         <v>20</v>
       </c>
-      <c r="F15" s="1">
-        <v>3</v>
-      </c>
-      <c r="G15" s="1">
-        <v>7</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K15" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1">
         <v>2019</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SUM(C16:G16)</f>
+        <v>23</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
         <v>7</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>3</v>
-      </c>
       <c r="K16" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1">
         <v>2019</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E17" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <f>SUM(C17:G17)</f>
+        <v>35</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="K17" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>2019</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f>SUM(C18:G18)</f>
+        <v>10</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1">
         <v>9</v>
       </c>
       <c r="K18" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>2019</v>
       </c>
       <c r="C19" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F19" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <f>SUM(C19:G19)</f>
+        <v>28</v>
       </c>
       <c r="I19" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J19" s="1">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="K19" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
         <v>2019</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>SUM(C20:G20)</f>
+        <v>4</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
       </c>
       <c r="J20" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K20" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>2019</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C21:G21)</f>
+        <v>10</v>
       </c>
       <c r="I21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K21" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>2019</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(C22:G22)</f>
+        <v>52</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="K22" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>2020</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
       <c r="E23" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>SUM(C23:G23)</f>
+        <v>24</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K23" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1">
         <v>2020</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>SUM(C24:G24)</f>
+        <v>26</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K24" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1">
         <v>2020</v>
       </c>
       <c r="C25" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G25" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>SUM(C25:G25)</f>
+        <v>42</v>
       </c>
       <c r="I25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K25" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2145,7 +2154,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C26:G26)</f>
         <v>36</v>
       </c>
       <c r="I26" s="2">
@@ -2158,8 +2167,546 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>8</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <f>SUM(C27:G27)</f>
+        <v>14</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+      <c r="K27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2">
+        <v>26</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3</v>
+      </c>
+      <c r="H28" s="2">
+        <f>SUM(C28:G28)</f>
+        <v>33</v>
+      </c>
+      <c r="I28" s="2">
+        <v>7</v>
+      </c>
+      <c r="J28" s="2">
+        <v>9</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C29" s="2">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>37</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2">
+        <f>SUM(C29:G29)</f>
+        <v>54</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5</v>
+      </c>
+      <c r="J29" s="2">
+        <v>25</v>
+      </c>
+      <c r="K29" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>7</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <f>SUM(C30:G30)</f>
+        <v>12</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2">
+        <v>3</v>
+      </c>
+      <c r="K30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2">
+        <v>22</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>6</v>
+      </c>
+      <c r="H31" s="2">
+        <f>SUM(C31:G31)</f>
+        <v>39</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>7</v>
+      </c>
+      <c r="K31" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2">
+        <v>25</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>4</v>
+      </c>
+      <c r="H32" s="2">
+        <f>SUM(C32:G32)</f>
+        <v>39</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>21</v>
+      </c>
+      <c r="K32" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C33" s="2">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2">
+        <v>12</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>4</v>
+      </c>
+      <c r="H33" s="2">
+        <f>SUM(C33:G33)</f>
+        <v>28</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>11</v>
+      </c>
+      <c r="K33" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>12</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <f>SUM(C34:G34)</f>
+        <v>12</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>12</v>
+      </c>
+      <c r="K34" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3</v>
+      </c>
+      <c r="E35" s="2">
+        <v>7</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+      <c r="H35" s="2">
+        <f>SUM(C35:G35)</f>
+        <v>11</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4</v>
+      </c>
+      <c r="K35" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C36" s="2">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2">
+        <v>11</v>
+      </c>
+      <c r="E36" s="2">
+        <v>29</v>
+      </c>
+      <c r="F36" s="2">
+        <v>7</v>
+      </c>
+      <c r="G36" s="2">
+        <v>10</v>
+      </c>
+      <c r="H36" s="2">
+        <f>SUM(C36:G36)</f>
+        <v>65</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2">
+        <v>40</v>
+      </c>
+      <c r="K36" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2">
+        <v>6</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>2</v>
+      </c>
+      <c r="H37" s="2">
+        <f>SUM(C37:G37)</f>
+        <v>13</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>3</v>
+      </c>
+      <c r="K37" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2">
+        <v>26</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>3</v>
+      </c>
+      <c r="H38" s="2">
+        <f>SUM(C38:G38)</f>
+        <v>33</v>
+      </c>
+      <c r="I38" s="2">
+        <v>7</v>
+      </c>
+      <c r="J38" s="2">
+        <v>9</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C39" s="2">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
+        <v>40</v>
+      </c>
+      <c r="F39" s="2">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2">
+        <v>3</v>
+      </c>
+      <c r="H39" s="2">
+        <f>SUM(C39:G39)</f>
+        <v>55</v>
+      </c>
+      <c r="I39" s="2">
+        <v>2</v>
+      </c>
+      <c r="J39" s="2">
+        <v>25</v>
+      </c>
+      <c r="K39" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <f>SUM(C40:G40)</f>
+        <v>14</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2</v>
+      </c>
+      <c r="K40" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C41" s="2">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2">
+        <v>7</v>
+      </c>
+      <c r="E41" s="2">
+        <v>19</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>5</v>
+      </c>
+      <c r="H41" s="2">
+        <f>SUM(C41:G41)</f>
+        <v>35</v>
+      </c>
+      <c r="I41" s="2">
+        <v>7</v>
+      </c>
+      <c r="J41" s="2">
+        <v>8</v>
+      </c>
+      <c r="K41" s="2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
docs: more 2021 data
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\PlanModels\saas-pricing\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57D1D5B-FBFC-4D98-8F7F-F60681BC5846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B6274B-1EE2-4FDA-952D-3E18C717A3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
@@ -1224,7 +1224,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K47" sqref="K47"/>
+      <selection pane="topRight" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
docs: more 2021 plans
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\practica\pgmarc\saas-pricing\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5846B009-C99A-4FFF-B06B-931795D9AFA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F4D903-00B3-4CC0-BC3A-B4DC96152093}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>saasName</t>
   </si>
@@ -882,8 +882,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K49" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K49" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K52" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K52" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}">
     <filterColumn colId="1">
       <filters>
         <filter val="2021"/>
@@ -1209,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J54" sqref="J54"/>
+      <selection pane="topRight" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2984,6 +2984,114 @@
         <v>4</v>
       </c>
     </row>
+    <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2</v>
+      </c>
+      <c r="D50" s="2">
+        <v>5</v>
+      </c>
+      <c r="E50" s="2">
+        <v>8</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>3</v>
+      </c>
+      <c r="H50" s="2">
+        <f>SUM(C50:G50)</f>
+        <v>18</v>
+      </c>
+      <c r="I50" s="2">
+        <v>2</v>
+      </c>
+      <c r="J50" s="2">
+        <v>2</v>
+      </c>
+      <c r="K50" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2">
+        <v>37</v>
+      </c>
+      <c r="F51" s="2">
+        <v>2</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2">
+        <f>SUM(C51:G51)</f>
+        <v>45</v>
+      </c>
+      <c r="I51" s="2">
+        <v>11</v>
+      </c>
+      <c r="J51" s="2">
+        <v>10</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C52" s="2">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2">
+        <v>4</v>
+      </c>
+      <c r="E52" s="2">
+        <v>40</v>
+      </c>
+      <c r="F52" s="2">
+        <v>2</v>
+      </c>
+      <c r="G52" s="2">
+        <v>3</v>
+      </c>
+      <c r="H52" s="2">
+        <f>SUM(C52:G52)</f>
+        <v>55</v>
+      </c>
+      <c r="I52" s="2">
+        <v>3</v>
+      </c>
+      <c r="J52" s="2">
+        <v>25</v>
+      </c>
+      <c r="K52" s="2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
FIX: RIPLING 2023 NUMBER OF ADDONS
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\PlanModels\saas-pricing\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/Trabajo/Técnico 2023 (corto)/saas-pricing/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AECC47C-0ECC-4C2A-AAD4-6861E02418BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E63D08-74FF-FD4A-B5FC-C30F40F5F6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1217,16 +1217,16 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A14" sqref="A14"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="11" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>50</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J11" s="1">
         <v>37</v>
@@ -1621,7 +1621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>15</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>21</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>14</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>16</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>12</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
docs: updated pricing data
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\PlanModels\saas-pricing\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AECC47C-0ECC-4C2A-AAD4-6861E02418BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F283DB-5B41-4203-8664-1131CCCDF83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>saasName</t>
   </si>
@@ -893,8 +893,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K53" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K53" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K56" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K56" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2023"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
     <sortCondition ref="A1:A53"/>
   </sortState>
@@ -1214,9 +1220,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A14" sqref="A14"/>
     </sheetView>
@@ -1729,7 +1735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1873,7 +1879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1909,7 +1915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1965,11 +1971,11 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -1978,10 +1984,10 @@
         <v>4</v>
       </c>
       <c r="K21" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -2086,10 +2092,10 @@
         <v>7</v>
       </c>
       <c r="K24" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2133,23 +2139,23 @@
         <v>2022</v>
       </c>
       <c r="C26" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F26" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G26" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -2158,10 +2164,10 @@
         <v>11</v>
       </c>
       <c r="K26" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="22.05" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2211,17 +2217,17 @@
         <v>4</v>
       </c>
       <c r="E28" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F28" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I28" s="2">
         <v>5</v>
@@ -2233,7 +2239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
@@ -2313,35 +2319,35 @@
         <v>2020</v>
       </c>
       <c r="C31" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" s="2">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F31" s="2">
         <v>2</v>
       </c>
       <c r="G31" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I31" s="2">
         <v>1</v>
       </c>
       <c r="J31" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K31" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -2377,7 +2383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -2421,13 +2427,13 @@
         <v>2020</v>
       </c>
       <c r="C34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
       </c>
       <c r="E34" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" s="2">
         <v>0</v>
@@ -2446,10 +2452,10 @@
         <v>4</v>
       </c>
       <c r="K34" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
@@ -2493,13 +2499,13 @@
         <v>2020</v>
       </c>
       <c r="C36" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E36" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -2509,7 +2515,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
@@ -2521,7 +2527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>55</v>
       </c>
       <c r="I38" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J38" s="2">
         <v>25</v>
@@ -2593,7 +2599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2701,7 +2707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>15</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>21</v>
       </c>
@@ -2889,13 +2895,13 @@
         <v>2021</v>
       </c>
       <c r="C47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2">
         <v>3</v>
       </c>
       <c r="E47" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" s="2">
         <v>0</v>
@@ -2914,10 +2920,10 @@
         <v>4</v>
       </c>
       <c r="K47" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>14</v>
       </c>
@@ -2953,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +2995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>16</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>12</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
@@ -3130,6 +3136,114 @@
         <v>11</v>
       </c>
       <c r="K53" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3</v>
+      </c>
+      <c r="D54" s="2">
+        <v>5</v>
+      </c>
+      <c r="E54" s="2">
+        <v>21</v>
+      </c>
+      <c r="F54" s="2">
+        <v>9</v>
+      </c>
+      <c r="G54" s="2">
+        <v>9</v>
+      </c>
+      <c r="H54" s="2">
+        <f>SUM(C54:G54)</f>
+        <v>47</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2">
+        <v>17</v>
+      </c>
+      <c r="K54" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>19</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2">
+        <v>7</v>
+      </c>
+      <c r="H55" s="2">
+        <f>SUM(C55:G55)</f>
+        <v>31</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2">
+        <v>12</v>
+      </c>
+      <c r="K55" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>5</v>
+      </c>
+      <c r="E56" s="2">
+        <v>8</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <f>SUM(C56:G56)</f>
+        <v>14</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2">
+        <v>3</v>
+      </c>
+      <c r="K56" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DOCS: NEW SAAS DATASET VERSION
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/Trabajo/Técnico 2023 (corto)/saas-pricing/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E63D08-74FF-FD4A-B5FC-C30F40F5F6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCE936C-88B7-6D4E-B123-2AD27956C0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
+    <workbookView xWindow="3040" yWindow="6240" windowWidth="23260" windowHeight="12580" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>saasName</t>
   </si>
@@ -893,8 +893,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K53" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K53" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K56" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K56" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
     <sortCondition ref="A1:A53"/>
   </sortState>
@@ -1214,11 +1214,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I11" sqref="I11"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1612,7 +1612,7 @@
         <v>50</v>
       </c>
       <c r="I11" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J11" s="1">
         <v>37</v>
@@ -1965,11 +1965,11 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -1978,7 +1978,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
         <v>7</v>
       </c>
       <c r="K24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -2133,23 +2133,23 @@
         <v>2022</v>
       </c>
       <c r="C26" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F26" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G26" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -2158,7 +2158,7 @@
         <v>11</v>
       </c>
       <c r="K26" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,17 +2211,17 @@
         <v>4</v>
       </c>
       <c r="E28" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F28" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I28" s="2">
         <v>5</v>
@@ -2313,29 +2313,29 @@
         <v>2020</v>
       </c>
       <c r="C31" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" s="2">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F31" s="2">
         <v>2</v>
       </c>
       <c r="G31" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I31" s="2">
         <v>1</v>
       </c>
       <c r="J31" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K31" s="2">
         <v>4</v>
@@ -2421,13 +2421,13 @@
         <v>2020</v>
       </c>
       <c r="C34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
       </c>
       <c r="E34" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" s="2">
         <v>0</v>
@@ -2446,7 +2446,7 @@
         <v>4</v>
       </c>
       <c r="K34" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="19" x14ac:dyDescent="0.25">
@@ -2493,13 +2493,13 @@
         <v>2020</v>
       </c>
       <c r="C36" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E36" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I36" s="2">
         <v>0</v>
@@ -2584,7 +2584,7 @@
         <v>55</v>
       </c>
       <c r="I38" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J38" s="2">
         <v>25</v>
@@ -2889,13 +2889,13 @@
         <v>2021</v>
       </c>
       <c r="C47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2">
         <v>3</v>
       </c>
       <c r="E47" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" s="2">
         <v>0</v>
@@ -2914,7 +2914,7 @@
         <v>4</v>
       </c>
       <c r="K47" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="19" x14ac:dyDescent="0.25">
@@ -3130,6 +3130,114 @@
         <v>11</v>
       </c>
       <c r="K53" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3</v>
+      </c>
+      <c r="D54" s="2">
+        <v>5</v>
+      </c>
+      <c r="E54" s="2">
+        <v>21</v>
+      </c>
+      <c r="F54" s="2">
+        <v>9</v>
+      </c>
+      <c r="G54" s="2">
+        <v>9</v>
+      </c>
+      <c r="H54" s="2">
+        <f>SUM(C54:G54)</f>
+        <v>47</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2">
+        <v>17</v>
+      </c>
+      <c r="K54" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>19</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2">
+        <v>7</v>
+      </c>
+      <c r="H55" s="2">
+        <f>SUM(C55:G55)</f>
+        <v>31</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2">
+        <v>12</v>
+      </c>
+      <c r="K55" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>5</v>
+      </c>
+      <c r="E56" s="2">
+        <v>8</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <f>SUM(C56:G56)</f>
+        <v>14</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2">
+        <v>3</v>
+      </c>
+      <c r="K56" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: ADDED MORE FEATURES TO DATASET
</commit_message>
<xml_diff>
--- a/datasets/pricingData.xlsx
+++ b/datasets/pricingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/Trabajo/Técnico 2023 (corto)/saas-pricing/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC07C55-C173-9E42-904B-D43D00B035B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2DCC16-0214-2140-A2FA-FEC7E3FDB1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{25F21780-5A2F-C44B-BBBA-624D4B9A13A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>saasName</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>numberOfPlans</t>
+  </si>
+  <si>
+    <t>guaranteeFeatures</t>
+  </si>
+  <si>
+    <t>supportFeatures</t>
+  </si>
+  <si>
+    <t>paymentFeatures</t>
   </si>
 </sst>
 </file>
@@ -342,7 +351,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -377,9 +428,85 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
@@ -893,25 +1020,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:K56" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K56" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}" name="pricingData" displayName="pricingData" ref="A1:N56" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:N56" xr:uid="{71575FB6-1D03-1C43-A1F5-34842B35C366}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N14">
     <sortCondition ref="A1:A53"/>
   </sortState>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{49B744FF-135F-FB49-8E67-3ADFF62F7F62}" name="informationFeatures" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{1B62A5E0-E167-3145-9233-957D202AC16A}" name="integrationFeatures" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{CEACD7F9-49A9-9E45-8D00-FFC8B5A30D0D}" name="toolFeatures" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{0222289F-50F8-9242-832F-7A98C3ED517F}" name="automationFeatures" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3195318E-BB70-0B45-A51D-5FD62E35192E}" name="managementFeatures" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5275409F-8C49-954E-A147-3656249FC072}" name="numberOfFeatures" dataDxfId="3">
-      <calculatedColumnFormula>SUM(C2:G2)</calculatedColumnFormula>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{67E661AB-ED78-E749-B7F6-2403E5761B9C}" name="saasName" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{F0FA794E-2A8D-B84A-B6E3-F7CB2E77A89D}" name="year" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{49B744FF-135F-FB49-8E67-3ADFF62F7F62}" name="informationFeatures" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{1B62A5E0-E167-3145-9233-957D202AC16A}" name="integrationFeatures" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{CEACD7F9-49A9-9E45-8D00-FFC8B5A30D0D}" name="toolFeatures" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{0222289F-50F8-9242-832F-7A98C3ED517F}" name="automationFeatures" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{3195318E-BB70-0B45-A51D-5FD62E35192E}" name="managementFeatures" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{1B5C3F87-58A0-D14F-A8F0-75D52E341D11}" name="guaranteeFeatures" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{5256040D-A619-3C49-B0BB-7800634C04CF}" name="supportFeatures" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{03706E74-4ADC-5141-8D7F-791A03D2F58F}" name="paymentFeatures" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{5275409F-8C49-954E-A147-3656249FC072}" name="numberOfFeatures" dataDxfId="0">
+      <calculatedColumnFormula>SUM(C2:J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{129E0E18-6600-354E-AD0E-5A7A34201D39}" name="numberOfAddOns" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{BFFF5A20-56DB-2A47-AB0B-063517490554}" name="numberOfCommonFeatures" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{7C71CB94-471E-4642-BC09-7715792BEAD6}" name="numberOfPlans" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{129E0E18-6600-354E-AD0E-5A7A34201D39}" name="numberOfAddOns" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{BFFF5A20-56DB-2A47-AB0B-063517490554}" name="numberOfCommonFeatures" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{7C71CB94-471E-4642-BC09-7715792BEAD6}" name="numberOfPlans" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1214,19 +1344,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F96C7FC-1D1C-C942-AA7C-1452045E2D1A}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L11" sqref="L11"/>
+      <selection pane="topRight" activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="38" customWidth="1"/>
+    <col min="1" max="14" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1249,19 +1379,28 @@
         <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1284,20 +1423,29 @@
         <v>7</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H14" si="0">SUM(C2:G2)</f>
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="10">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2:K56" si="0">SUM(C2:J2)</f>
+        <v>61</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10">
         <v>19</v>
       </c>
-      <c r="K2" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1320,20 +1468,29 @@
         <v>26</v>
       </c>
       <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
         <v>23</v>
       </c>
-      <c r="K3" s="1">
+      <c r="N3" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1356,20 +1513,29 @@
         <v>10</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="L4" s="1">
         <v>5</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>19</v>
       </c>
-      <c r="K4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1392,20 +1558,29 @@
         <v>6</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>2</v>
       </c>
       <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1">
         <v>37</v>
       </c>
-      <c r="K5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1428,20 +1603,29 @@
         <v>16</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
         <v>15</v>
       </c>
-      <c r="K6" s="1">
+      <c r="N6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1464,20 +1648,29 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
         <v>8</v>
       </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>8</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="N7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1500,20 +1693,29 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>3</v>
+      </c>
+      <c r="N8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1536,20 +1738,29 @@
         <v>14</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="1">
         <v>44</v>
       </c>
-      <c r="K9" s="1">
+      <c r="N9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1572,20 +1783,29 @@
         <v>8</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4</v>
+      </c>
+      <c r="M10" s="1">
         <v>7</v>
       </c>
-      <c r="K10" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1608,20 +1828,29 @@
         <v>7</v>
       </c>
       <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="I11" s="1">
+      <c r="L11" s="1">
         <v>13</v>
       </c>
-      <c r="J11" s="1">
+      <c r="M11" s="1">
         <v>37</v>
       </c>
-      <c r="K11" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1644,20 +1873,29 @@
         <v>4</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="L12" s="1">
         <v>6</v>
       </c>
-      <c r="J12" s="1">
+      <c r="M12" s="1">
         <v>25</v>
       </c>
-      <c r="K12" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1680,20 +1918,29 @@
         <v>2</v>
       </c>
       <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
         <v>8</v>
       </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1716,20 +1963,29 @@
         <v>9</v>
       </c>
       <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="I14" s="1">
-        <v>4</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="L14" s="1">
+        <v>4</v>
+      </c>
+      <c r="M14" s="1">
         <v>22</v>
       </c>
-      <c r="K14" s="1">
+      <c r="N14" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1752,20 +2008,29 @@
         <v>2</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15:H40" si="1">SUM(C15:G15)</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1788,20 +2053,29 @@
         <v>6</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
         <v>7</v>
       </c>
-      <c r="K16" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1824,20 +2098,29 @@
         <v>7</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="1"/>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
         <v>7</v>
       </c>
-      <c r="K17" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1860,20 +2143,29 @@
         <v>1</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
       </c>
       <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
         <v>9</v>
       </c>
-      <c r="K18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1896,20 +2188,29 @@
         <v>3</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
         <v>9</v>
       </c>
-      <c r="K19" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1932,20 +2233,29 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
       </c>
       <c r="J20" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K20" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>4</v>
+      </c>
+      <c r="N20" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1968,20 +2278,29 @@
         <v>1</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K21" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>4</v>
+      </c>
+      <c r="N21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -2004,20 +2323,29 @@
         <v>2</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="1"/>
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
         <v>37</v>
       </c>
-      <c r="K22" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2040,20 +2368,29 @@
         <v>4</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <v>10</v>
       </c>
-      <c r="K23" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -2076,20 +2413,29 @@
         <v>8</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
         <v>7</v>
       </c>
-      <c r="K24" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -2112,20 +2458,29 @@
         <v>9</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
         <v>18</v>
       </c>
-      <c r="K25" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2148,20 +2503,29 @@
         <v>7</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="1"/>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="I26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
         <v>11</v>
       </c>
-      <c r="K26" s="2">
+      <c r="N26" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
@@ -2184,20 +2548,29 @@
         <v>1</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I27" s="2">
         <v>1</v>
       </c>
       <c r="J27" s="2">
-        <v>2</v>
-      </c>
-      <c r="K27" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2">
+        <v>2</v>
+      </c>
+      <c r="N27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2220,20 +2593,29 @@
         <v>3</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="I28" s="2">
+      <c r="L28" s="2">
         <v>5</v>
       </c>
-      <c r="J28" s="2">
+      <c r="M28" s="2">
         <v>25</v>
       </c>
-      <c r="K28" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N28" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -2256,20 +2638,29 @@
         <v>1</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
       </c>
       <c r="J29" s="2">
-        <v>3</v>
-      </c>
-      <c r="K29" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2">
+        <v>3</v>
+      </c>
+      <c r="N29" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
@@ -2292,20 +2683,29 @@
         <v>6</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="I30" s="2">
         <v>0</v>
       </c>
       <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2">
         <v>7</v>
       </c>
-      <c r="K30" s="2">
+      <c r="N30" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
@@ -2328,20 +2728,29 @@
         <v>1</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="I31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
         <v>22</v>
       </c>
-      <c r="K31" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N31" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -2364,20 +2773,29 @@
         <v>4</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="I32" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
         <v>11</v>
       </c>
-      <c r="K32" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N32" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
@@ -2400,20 +2818,29 @@
         <v>0</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2">
         <v>12</v>
       </c>
-      <c r="I33" s="2">
-        <v>0</v>
-      </c>
-      <c r="J33" s="2">
-        <v>12</v>
-      </c>
-      <c r="K33" s="2">
+      <c r="N33" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -2436,20 +2863,29 @@
         <v>1</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="2">
-        <v>4</v>
-      </c>
-      <c r="K34" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2">
+        <v>4</v>
+      </c>
+      <c r="N34" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
@@ -2472,20 +2908,29 @@
         <v>10</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="1"/>
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="I35" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="L35" s="2">
+        <v>2</v>
+      </c>
+      <c r="M35" s="2">
         <v>40</v>
       </c>
-      <c r="K35" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N35" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
@@ -2508,20 +2953,29 @@
         <v>2</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I36" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J36" s="2">
-        <v>3</v>
-      </c>
-      <c r="K36" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2">
+        <v>3</v>
+      </c>
+      <c r="N36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -2544,20 +2998,29 @@
         <v>3</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="L37" s="2">
         <v>7</v>
       </c>
-      <c r="J37" s="2">
+      <c r="M37" s="2">
         <v>9</v>
       </c>
-      <c r="K37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -2580,20 +3043,29 @@
         <v>3</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="I38" s="2">
+      <c r="L38" s="2">
         <v>11</v>
       </c>
-      <c r="J38" s="2">
+      <c r="M38" s="2">
         <v>25</v>
       </c>
-      <c r="K38" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N38" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
@@ -2616,20 +3088,29 @@
         <v>1</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="I39" s="2">
-        <v>0</v>
-      </c>
-      <c r="J39" s="2">
-        <v>2</v>
-      </c>
-      <c r="K39" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <v>2</v>
+      </c>
+      <c r="N39" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
@@ -2652,20 +3133,29 @@
         <v>5</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="I40" s="2">
+      <c r="L40" s="2">
         <v>7</v>
       </c>
-      <c r="J40" s="2">
+      <c r="M40" s="2">
         <v>8</v>
       </c>
-      <c r="K40" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N40" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2688,20 +3178,29 @@
         <v>4</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" ref="H41:H46" si="2">SUM(C41:G41)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="I41" s="2">
-        <v>0</v>
-      </c>
-      <c r="J41" s="2">
+      <c r="L41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
         <v>10</v>
       </c>
-      <c r="K41" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N41" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
@@ -2724,20 +3223,29 @@
         <v>7</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0</v>
+      </c>
+      <c r="M42" s="2">
         <v>6</v>
       </c>
-      <c r="K42" s="2">
+      <c r="N42" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
@@ -2760,20 +3268,29 @@
         <v>9</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="2"/>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J43" s="2">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0</v>
+      </c>
+      <c r="M43" s="2">
         <v>17</v>
       </c>
-      <c r="K43" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N43" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -2796,20 +3313,29 @@
         <v>7</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="I44" s="2">
         <v>1</v>
       </c>
       <c r="J44" s="2">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L44" s="2">
+        <v>1</v>
+      </c>
+      <c r="M44" s="2">
         <v>12</v>
       </c>
-      <c r="K44" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N44" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>15</v>
       </c>
@@ -2832,20 +3358,29 @@
         <v>11</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="I45" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="L45" s="2">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2">
         <v>16</v>
       </c>
-      <c r="K45" s="2">
+      <c r="N45" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
@@ -2868,20 +3403,29 @@
         <v>0</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="2">
+        <v>1</v>
+      </c>
+      <c r="K46" s="1">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="K46" s="2">
+      <c r="L46" s="2">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2">
+        <v>16</v>
+      </c>
+      <c r="N46" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>21</v>
       </c>
@@ -2904,20 +3448,29 @@
         <v>1</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" ref="H47:H53" si="3">SUM(C47:G47)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="2">
-        <v>4</v>
-      </c>
-      <c r="K47" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0</v>
+      </c>
+      <c r="M47" s="2">
+        <v>4</v>
+      </c>
+      <c r="N47" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>14</v>
       </c>
@@ -2940,20 +3493,29 @@
         <v>11</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="3"/>
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="I48" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="L48" s="2">
+        <v>2</v>
+      </c>
+      <c r="M48" s="2">
         <v>41</v>
       </c>
-      <c r="K48" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N48" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
@@ -2970,26 +3532,35 @@
         <v>8</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G49" s="2">
         <v>3</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="3"/>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="I49" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" s="2">
-        <v>2</v>
-      </c>
-      <c r="K49" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K49" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="L49" s="2">
+        <v>2</v>
+      </c>
+      <c r="M49" s="2">
+        <v>2</v>
+      </c>
+      <c r="N49" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
@@ -3012,20 +3583,29 @@
         <v>1</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="I50" s="2">
+      <c r="L50" s="2">
         <v>7</v>
       </c>
-      <c r="J50" s="2">
+      <c r="M50" s="2">
         <v>10</v>
       </c>
-      <c r="K50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>16</v>
       </c>
@@ -3048,20 +3628,29 @@
         <v>3</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="I51" s="2">
+      <c r="L51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="2">
+      <c r="M51" s="2">
         <v>25</v>
       </c>
-      <c r="K51" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N51" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>12</v>
       </c>
@@ -3084,20 +3673,29 @@
         <v>1</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I52" s="2">
-        <v>0</v>
-      </c>
-      <c r="J52" s="2">
-        <v>2</v>
-      </c>
-      <c r="K52" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="L52" s="2">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2">
+        <v>2</v>
+      </c>
+      <c r="N52" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>19</v>
       </c>
@@ -3120,20 +3718,29 @@
         <v>6</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0</v>
+      </c>
+      <c r="K53" s="1">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="I53" s="2">
-        <v>4</v>
-      </c>
-      <c r="J53" s="2">
+      <c r="L53" s="2">
+        <v>4</v>
+      </c>
+      <c r="M53" s="2">
         <v>11</v>
       </c>
-      <c r="K53" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N53" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>10</v>
       </c>
@@ -3156,20 +3763,29 @@
         <v>9</v>
       </c>
       <c r="H54" s="2">
-        <f>SUM(C54:G54)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="I54" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J54" s="2">
+        <v>1</v>
+      </c>
+      <c r="K54" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="L54" s="2">
+        <v>0</v>
+      </c>
+      <c r="M54" s="2">
         <v>17</v>
       </c>
-      <c r="K54" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N54" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>17</v>
       </c>
@@ -3192,20 +3808,29 @@
         <v>7</v>
       </c>
       <c r="H55" s="2">
-        <f>SUM(C55:G55)</f>
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="I55" s="2">
         <v>1</v>
       </c>
       <c r="J55" s="2">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="L55" s="2">
+        <v>1</v>
+      </c>
+      <c r="M55" s="2">
         <v>12</v>
       </c>
-      <c r="K55" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="N55" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>21</v>
       </c>
@@ -3228,16 +3853,25 @@
         <v>0</v>
       </c>
       <c r="H56" s="2">
-        <f>SUM(C56:G56)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" s="2">
-        <v>3</v>
-      </c>
-      <c r="K56" s="2">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2">
+        <v>3</v>
+      </c>
+      <c r="N56" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>